<commit_message>
ya funca que se mantengan las formulas, falta agregar test y ver el tema del style de la pestaña de resumen de compra
</commit_message>
<xml_diff>
--- a/Pedidos/2021/012020/Generador de pedidos/Generador de pedidos.xlsx
+++ b/Pedidos/2021/012020/Generador de pedidos/Generador de pedidos.xlsx
@@ -46,6 +46,9 @@
     <t xml:space="preserve">Test con combo (OJO LA CANTIDAD QUE DICE LA TENES QUE MULTIPLICARLA)</t>
   </si>
   <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
     <t xml:space="preserve">PEDIDO: TIE-G0DXY
 — [ 2 ] BBQ Ribs Guarnición: Puré de papas &gt; $ 780,00
 Total: $ 780,00
@@ -153,9 +156,6 @@
   </si>
   <si>
     <t xml:space="preserve">Bien hecho retiro en local. DEJAR ESTOS ULTIMOS DOS TESTS PARA EL FINAL (retiro en local puede traer problemas)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
   </si>
   <si>
     <r>
@@ -175,6 +175,7 @@
         <color rgb="FF000000"/>
         <rFont val="Cambria"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[ 2 ] </t>
     </r>
@@ -293,6 +294,7 @@
       <color rgb="FF000000"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -389,11 +391,11 @@
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.40234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="90.13"/>
@@ -423,13 +425,13 @@
     </row>
     <row r="3" customFormat="false" ht="149.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="162.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -437,10 +439,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="176.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -448,10 +450,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="202.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -459,10 +461,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="216.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -470,10 +472,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="270.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -481,10 +483,10 @@
         <v>2</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="283.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -492,15 +494,15 @@
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="141" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>20</v>
@@ -1518,7 +1520,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="77.93"/>
   </cols>
@@ -1533,7 +1535,7 @@
     </row>
     <row r="2" customFormat="false" ht="177.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>21</v>
@@ -1541,7 +1543,7 @@
     </row>
     <row r="3" customFormat="false" ht="128.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>22</v>
@@ -1549,7 +1551,7 @@
     </row>
     <row r="4" customFormat="false" ht="141" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>23</v>
@@ -1557,7 +1559,7 @@
     </row>
     <row r="5" customFormat="false" ht="153.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>24</v>
@@ -1565,7 +1567,7 @@
     </row>
     <row r="6" customFormat="false" ht="128.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>25</v>

</xml_diff>